<commit_message>
changes before AP takes over
</commit_message>
<xml_diff>
--- a/FieldConfigrationFile.xlsx
+++ b/FieldConfigrationFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prakhar\Desktop\Projects\IMGC Project\Field Level Mapping Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Deepseek\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C0B099-C77B-42A8-AD99-0E551569F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D70DE7-6914-4810-802D-F13122B54DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{02CFE6FC-DC13-4DF7-B179-54CE07624848}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{02CFE6FC-DC13-4DF7-B179-54CE07624848}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="253">
   <si>
     <t>PAS Field Name</t>
   </si>
@@ -439,79 +439,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">In the PD document, the value can be extracted from the field </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Application No.”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> positioned just below the Personal Discussion Report header. This value typically appears as a 10-digit numeric identifier (e.g., 300002010).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">It can be found in the Application Form under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> “</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Application Form Number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,” usually shown at the top of the document. This value generally appears as a 10-digit numeric identifier (e.g., 300002010) and must be cross-validated with the corresponding 10-digit number in the email subject.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">It can be obtained from the Application Form under the </t>
     </r>
     <r>
@@ -11511,6 +11438,82 @@
   </si>
   <si>
     <t>Technical Report</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It can be found in the Application Form under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> “</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application Form Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,” usually shown at the top of the document. This value generally appears as a 10-character alpha numeric identifier (e.g., 300002010) and ideally should  be cross-validated with the corresponding 10-character alpha numeric  in the email subject.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the PD document, the value can be extracted from the field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Application No.”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> positioned just below the Personal Discussion Report header. This value typically appears as a 10-character alpha  numeric identifier (e.g., 300002010).</t>
+    </r>
+  </si>
+  <si>
+    <t>This value can be extracted from the Email Subject, where it typically appears as a 10-digit numeric identifier (e.g., 300002010).It may or may not be at the end of complete subject line.</t>
   </si>
 </sst>
 </file>
@@ -11611,7 +11614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -11628,16 +11631,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -11982,9 +11982,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3765008E-87C2-42DA-8C71-BC2650E30679}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12049,11 +12049,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="4" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="4" customFormat="1" ht="108" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C2" s="6">
@@ -12063,31 +12063,33 @@
         <v>127</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="10"/>
     </row>
     <row r="3" spans="1:14" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C3" s="6">
@@ -12097,25 +12099,25 @@
         <v>127</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
     </row>
     <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C4" s="6">
@@ -12125,31 +12127,31 @@
         <v>127</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="N4" s="10"/>
+      <c r="N4" s="9"/>
     </row>
     <row r="5" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C5" s="6">
@@ -12159,31 +12161,31 @@
         <v>127</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="N5" s="10"/>
+      <c r="N5" s="9"/>
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C6" s="6">
@@ -12193,25 +12195,25 @@
         <v>127</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F6" s="8"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
     </row>
     <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C7" s="6">
@@ -12221,33 +12223,33 @@
         <v>127</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="G7" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="N7" s="10"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="6">
@@ -12257,33 +12259,33 @@
         <v>127</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="G8" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="N8" s="10"/>
+      <c r="N8" s="9"/>
     </row>
     <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C9" s="6">
@@ -12293,29 +12295,29 @@
         <v>127</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C10" s="6">
@@ -12325,31 +12327,31 @@
         <v>127</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G10" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
     </row>
     <row r="11" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C11" s="6">
@@ -12359,33 +12361,33 @@
         <v>127</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G11" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="I11" s="10" t="s">
+      <c r="H11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I11" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
+      <c r="J11" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
     </row>
     <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C12" s="6">
@@ -12395,29 +12397,29 @@
         <v>127</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
     </row>
     <row r="13" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C13" s="6">
@@ -12427,29 +12429,29 @@
         <v>127</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+        <v>246</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
     </row>
     <row r="14" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C14" s="6">
@@ -12459,29 +12461,29 @@
         <v>127</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+        <v>246</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
     </row>
     <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>106</v>
       </c>
       <c r="C15" s="6">
@@ -12491,25 +12493,25 @@
         <v>127</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F15" s="8"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
     </row>
     <row r="16" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C16" s="6">
@@ -12519,29 +12521,29 @@
         <v>127</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
     </row>
     <row r="17" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>107</v>
       </c>
       <c r="C17" s="6">
@@ -12551,25 +12553,25 @@
         <v>128</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F17" s="8"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
     </row>
     <row r="18" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C18" s="6">
@@ -12579,25 +12581,25 @@
         <v>127</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F18" s="8"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
     </row>
     <row r="19" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C19" s="6">
@@ -12607,25 +12609,25 @@
         <v>127</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F19" s="8"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
     </row>
     <row r="20" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="6">
@@ -12635,1979 +12637,1979 @@
         <v>127</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F20" s="8"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
     </row>
     <row r="21" spans="1:14" ht="36" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>112</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
     </row>
     <row r="22" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="10">
         <v>0</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E22" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10" t="s">
+      <c r="G22" s="9"/>
+      <c r="H22" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="J22" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
     </row>
     <row r="23" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="10">
         <v>40</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F23" s="8"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
     </row>
     <row r="24" spans="1:14" ht="36" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="10">
         <v>0</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F24" s="8"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="10">
         <v>0</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E25" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10" t="s">
+      <c r="G25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J25" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
     </row>
     <row r="26" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="10">
         <v>0</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F26" s="8"/>
-      <c r="G26" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
+      <c r="G26" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
     </row>
     <row r="27" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="10">
         <v>0</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F27" s="8"/>
-      <c r="G27" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
+      <c r="G27" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
     </row>
     <row r="28" spans="1:14" ht="108" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="10">
         <v>22</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="J28" s="10" t="s">
-        <v>174</v>
-      </c>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
     </row>
     <row r="29" spans="1:14" ht="132" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="10">
         <v>0</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10" t="s">
+      <c r="G29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="J29" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="10">
         <v>0</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E30" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="10">
         <v>0</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
+        <v>246</v>
+      </c>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
     </row>
     <row r="32" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="10">
         <v>0</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
     </row>
     <row r="33" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>113</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
+        <v>246</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
     </row>
     <row r="34" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="10">
         <v>3</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="I34" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
     </row>
     <row r="35" spans="1:14" ht="132" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="10">
         <v>8</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
     </row>
     <row r="36" spans="1:14" ht="156" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="10">
         <v>3</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G36" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
     </row>
     <row r="37" spans="1:14" ht="132" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="10">
         <v>18</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="10"/>
-      <c r="L37" s="10"/>
-      <c r="M37" s="10"/>
-      <c r="N37" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
     </row>
     <row r="38" spans="1:14" ht="132" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="10">
         <v>18</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
     </row>
     <row r="39" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="10">
         <v>18</v>
       </c>
       <c r="D39" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
     </row>
     <row r="40" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="10">
         <v>20</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
+        <v>246</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
     </row>
     <row r="41" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
-      <c r="M41" s="10"/>
-      <c r="N41" s="10"/>
+      <c r="G41" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
     </row>
     <row r="42" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F42" s="8"/>
-      <c r="G42" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
+      <c r="G42" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
     </row>
     <row r="43" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>115</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
     </row>
     <row r="44" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="10" t="s">
         <v>115</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="H44" s="10"/>
-      <c r="I44" s="10"/>
-      <c r="J44" s="10"/>
-      <c r="K44" s="10"/>
-      <c r="L44" s="10"/>
-      <c r="M44" s="10"/>
-      <c r="N44" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
     </row>
     <row r="45" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>115</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F45" s="8"/>
-      <c r="G45" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="10"/>
-      <c r="K45" s="10"/>
-      <c r="L45" s="10"/>
-      <c r="M45" s="10"/>
-      <c r="N45" s="10"/>
+      <c r="G45" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
     </row>
     <row r="46" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="10">
         <v>0</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F46" s="8"/>
-      <c r="G46" s="10"/>
-      <c r="H46" s="10"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="10"/>
-      <c r="K46" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="L46" s="10"/>
-      <c r="M46" s="10"/>
-      <c r="N46" s="10"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
     </row>
     <row r="47" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="10">
         <v>0</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F47" s="8"/>
-      <c r="G47" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="H47" s="10"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="10"/>
-      <c r="K47" s="10"/>
-      <c r="L47" s="10"/>
-      <c r="M47" s="10"/>
-      <c r="N47" s="10"/>
+      <c r="G47" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
     </row>
     <row r="48" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F48" s="8"/>
-      <c r="G48" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="H48" s="10"/>
-      <c r="I48" s="10"/>
-      <c r="J48" s="10"/>
-      <c r="K48" s="10"/>
-      <c r="L48" s="10"/>
-      <c r="M48" s="10"/>
-      <c r="N48" s="10"/>
+      <c r="G48" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
     </row>
     <row r="49" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="10" t="s">
         <v>116</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="H49" s="10"/>
-      <c r="I49" s="10"/>
-      <c r="J49" s="10"/>
-      <c r="K49" s="10"/>
-      <c r="L49" s="10"/>
-      <c r="M49" s="10"/>
-      <c r="N49" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
     </row>
     <row r="50" spans="1:14" ht="132" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="10">
         <v>500</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="K50" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="L50" s="10"/>
-      <c r="M50" s="10"/>
-      <c r="N50" s="10"/>
+        <v>248</v>
+      </c>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
     </row>
     <row r="51" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="10">
         <v>0</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F51" s="8"/>
-      <c r="G51" s="10"/>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
-      <c r="K51" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="L51" s="10"/>
-      <c r="M51" s="10"/>
-      <c r="N51" s="10"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
     </row>
     <row r="52" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E52" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F52" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="10" t="s">
+      <c r="G52" s="9"/>
+      <c r="H52" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I52" s="10"/>
-      <c r="J52" s="10" t="s">
+      <c r="I52" s="9"/>
+      <c r="J52" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="K52" s="10"/>
-      <c r="L52" s="10"/>
-      <c r="M52" s="10"/>
-      <c r="N52" s="10"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
     </row>
     <row r="53" spans="1:14" ht="36" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F53" s="8"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="K53" s="10"/>
-      <c r="L53" s="10"/>
-      <c r="M53" s="10"/>
-      <c r="N53" s="10"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
     </row>
     <row r="54" spans="1:14" ht="108" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>113</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E54" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F54" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G54" s="10"/>
-      <c r="H54" s="10" t="s">
+      <c r="G54" s="9"/>
+      <c r="H54" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I54" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J54" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="K54" s="10"/>
-      <c r="L54" s="10"/>
-      <c r="M54" s="10"/>
-      <c r="N54" s="10"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
     </row>
     <row r="55" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="10" t="s">
         <v>118</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E55" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F55" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G55" s="10"/>
-      <c r="H55" s="10" t="s">
+      <c r="G55" s="9"/>
+      <c r="H55" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="I55" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="J55" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="I55" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="K55" s="10"/>
-      <c r="L55" s="10"/>
-      <c r="M55" s="10"/>
-      <c r="N55" s="10"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
     </row>
     <row r="56" spans="1:14" ht="108" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>119</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F56" s="8"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="I56" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
-      <c r="M56" s="10"/>
-      <c r="N56" s="10"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="I56" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
     </row>
     <row r="57" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E57" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F57" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F57" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G57" s="10"/>
-      <c r="H57" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="I57" s="10"/>
-      <c r="J57" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
-      <c r="M57" s="10"/>
-      <c r="N57" s="10"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
     </row>
     <row r="58" spans="1:14" ht="144" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="10" t="s">
         <v>118</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E58" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F58" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G58" s="10"/>
-      <c r="H58" s="10" t="s">
+      <c r="G58" s="9"/>
+      <c r="H58" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="J58" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="J58" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="K58" s="10"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
     </row>
     <row r="59" spans="1:14" ht="144" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>118</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E59" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="F59" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="F59" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G59" s="10"/>
-      <c r="H59" s="10" t="s">
+      <c r="G59" s="9"/>
+      <c r="H59" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J59" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="I59" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="K59" s="10"/>
-      <c r="L59" s="10"/>
-      <c r="M59" s="10"/>
-      <c r="N59" s="10"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
     </row>
     <row r="60" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C60" s="11">
+      <c r="C60" s="10">
         <v>80</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F60" s="8"/>
-      <c r="G60" s="10"/>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10"/>
-      <c r="J60" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="K60" s="10"/>
-      <c r="L60" s="10"/>
-      <c r="M60" s="10"/>
-      <c r="N60" s="10"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
     </row>
     <row r="61" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C61" s="11">
+      <c r="C61" s="10">
         <v>80</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F61" s="8"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="K61" s="10"/>
-      <c r="L61" s="10"/>
-      <c r="M61" s="10"/>
-      <c r="N61" s="10"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
     </row>
     <row r="62" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="10" t="s">
         <v>113</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F62" s="8"/>
-      <c r="G62" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="H62" s="10"/>
-      <c r="I62" s="10"/>
-      <c r="J62" s="10"/>
-      <c r="K62" s="10"/>
-      <c r="L62" s="10"/>
-      <c r="M62" s="10"/>
-      <c r="N62" s="10"/>
+      <c r="G62" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
     </row>
     <row r="63" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="10">
         <v>3</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="G63" s="10"/>
-      <c r="H63" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="I63" s="10"/>
-      <c r="J63" s="10"/>
-      <c r="K63" s="10"/>
-      <c r="L63" s="10"/>
-      <c r="M63" s="10"/>
-      <c r="N63" s="10"/>
+        <v>246</v>
+      </c>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
     </row>
     <row r="64" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C64" s="10" t="s">
         <v>117</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G64" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="H64" s="10"/>
-      <c r="I64" s="10"/>
-      <c r="J64" s="10"/>
-      <c r="K64" s="10"/>
-      <c r="L64" s="10"/>
-      <c r="M64" s="10"/>
-      <c r="N64" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
     </row>
     <row r="65" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="10" t="s">
         <v>120</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G65" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="H65" s="10"/>
-      <c r="I65" s="10"/>
-      <c r="J65" s="10"/>
-      <c r="K65" s="10"/>
-      <c r="L65" s="10"/>
-      <c r="M65" s="10"/>
-      <c r="N65" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
     </row>
     <row r="66" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C66" s="11" t="s">
+      <c r="C66" s="10" t="s">
         <v>120</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G66" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="H66" s="10"/>
-      <c r="I66" s="10"/>
-      <c r="J66" s="10"/>
-      <c r="K66" s="10"/>
-      <c r="L66" s="10"/>
-      <c r="M66" s="10"/>
-      <c r="N66" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
     </row>
     <row r="67" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="10" t="s">
         <v>121</v>
       </c>
       <c r="D67" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G67" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="H67" s="10"/>
-      <c r="I67" s="10"/>
-      <c r="J67" s="10"/>
-      <c r="K67" s="10"/>
-      <c r="L67" s="10"/>
-      <c r="M67" s="10"/>
-      <c r="N67" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
     </row>
     <row r="68" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="11">
+      <c r="C68" s="10">
         <v>18</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G68" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="H68" s="10"/>
-      <c r="I68" s="10"/>
-      <c r="J68" s="10"/>
-      <c r="K68" s="10"/>
-      <c r="L68" s="10"/>
-      <c r="M68" s="10"/>
-      <c r="N68" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
     </row>
     <row r="69" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="10" t="s">
         <v>121</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G69" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="H69" s="10"/>
-      <c r="I69" s="10"/>
-      <c r="J69" s="10"/>
-      <c r="K69" s="10"/>
-      <c r="L69" s="10"/>
-      <c r="M69" s="10"/>
-      <c r="N69" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
     </row>
     <row r="70" spans="1:14" ht="108" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C70" s="11">
+      <c r="C70" s="10">
         <v>18</v>
       </c>
       <c r="D70" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10"/>
-      <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
-      <c r="M70" s="10"/>
-      <c r="N70" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
     </row>
     <row r="71" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C71" s="10" t="s">
         <v>121</v>
       </c>
       <c r="D71" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
-      <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
-      <c r="M71" s="10"/>
-      <c r="N71" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G71" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
     </row>
     <row r="72" spans="1:14" ht="48" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="11">
+      <c r="C72" s="10">
         <v>16</v>
       </c>
       <c r="D72" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G72" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H72" s="10"/>
-      <c r="I72" s="10"/>
-      <c r="J72" s="10"/>
-      <c r="K72" s="10"/>
-      <c r="L72" s="10"/>
-      <c r="M72" s="10"/>
-      <c r="N72" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G72" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
     </row>
     <row r="73" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C73" s="10" t="s">
         <v>120</v>
       </c>
       <c r="D73" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="H73" s="10"/>
-      <c r="I73" s="10"/>
-      <c r="J73" s="10"/>
-      <c r="K73" s="10"/>
-      <c r="L73" s="10"/>
-      <c r="M73" s="10"/>
-      <c r="N73" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
     </row>
     <row r="74" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C74" s="11">
+      <c r="C74" s="10">
         <v>18</v>
       </c>
       <c r="D74" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G74" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H74" s="10"/>
-      <c r="I74" s="10"/>
-      <c r="J74" s="10"/>
-      <c r="K74" s="10"/>
-      <c r="L74" s="10"/>
-      <c r="M74" s="10"/>
-      <c r="N74" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
     </row>
     <row r="75" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C75" s="11">
+      <c r="C75" s="10">
         <v>16</v>
       </c>
       <c r="D75" s="8" t="s">
         <v>127</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="H75" s="10"/>
-      <c r="I75" s="10"/>
-      <c r="J75" s="10"/>
-      <c r="K75" s="10"/>
-      <c r="L75" s="10"/>
-      <c r="M75" s="10"/>
-      <c r="N75" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G75" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
     </row>
     <row r="76" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C76" s="11">
+      <c r="C76" s="10">
         <v>18</v>
       </c>
       <c r="D76" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G76" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="H76" s="10"/>
-      <c r="I76" s="10"/>
-      <c r="J76" s="10"/>
-      <c r="K76" s="10"/>
-      <c r="L76" s="10"/>
-      <c r="M76" s="10"/>
-      <c r="N76" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
     </row>
     <row r="77" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="10" t="s">
         <v>122</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H77" s="10"/>
-      <c r="I77" s="10"/>
-      <c r="J77" s="10"/>
-      <c r="K77" s="10"/>
-      <c r="L77" s="10"/>
-      <c r="M77" s="10"/>
-      <c r="N77" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
     </row>
     <row r="78" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="10" t="s">
         <v>114</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F78" s="8"/>
-      <c r="G78" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="H78" s="10"/>
-      <c r="I78" s="10"/>
-      <c r="J78" s="10"/>
-      <c r="K78" s="10"/>
-      <c r="L78" s="10"/>
-      <c r="M78" s="10"/>
-      <c r="N78" s="10"/>
+      <c r="G78" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
     </row>
     <row r="79" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C79" s="11">
+      <c r="C79" s="10">
         <v>0</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F79" s="8"/>
-      <c r="G79" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H79" s="10"/>
-      <c r="I79" s="10"/>
-      <c r="J79" s="10"/>
-      <c r="K79" s="10"/>
-      <c r="L79" s="10"/>
-      <c r="M79" s="10"/>
-      <c r="N79" s="10"/>
+      <c r="G79" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
     </row>
     <row r="80" spans="1:14" ht="72" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="11">
+      <c r="C80" s="10">
         <v>20</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F80" s="8"/>
-      <c r="G80" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="H80" s="10"/>
-      <c r="I80" s="10"/>
-      <c r="J80" s="10"/>
-      <c r="K80" s="10"/>
-      <c r="L80" s="10"/>
-      <c r="M80" s="10"/>
-      <c r="N80" s="10"/>
+      <c r="G80" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
     </row>
     <row r="81" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C81" s="11">
+      <c r="C81" s="10">
         <v>0</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F81" s="8"/>
-      <c r="G81" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H81" s="10"/>
-      <c r="I81" s="10"/>
-      <c r="J81" s="10"/>
-      <c r="K81" s="10"/>
-      <c r="L81" s="10"/>
-      <c r="M81" s="10"/>
-      <c r="N81" s="10"/>
+      <c r="G81" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
     </row>
     <row r="82" spans="1:14" ht="84" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C82" s="11" t="s">
+      <c r="C82" s="10" t="s">
         <v>121</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="H82" s="10"/>
-      <c r="I82" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="J82" s="10"/>
-      <c r="K82" s="10"/>
-      <c r="L82" s="10"/>
-      <c r="M82" s="10"/>
-      <c r="N82" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G82" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
     </row>
     <row r="83" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C83" s="11">
+      <c r="C83" s="10">
         <v>18</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="H83" s="10"/>
-      <c r="I83" s="10"/>
-      <c r="J83" s="10"/>
-      <c r="K83" s="10"/>
-      <c r="L83" s="10"/>
-      <c r="M83" s="10"/>
-      <c r="N83" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="9"/>
     </row>
     <row r="84" spans="1:14" ht="96" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C84" s="11">
+      <c r="C84" s="10">
         <v>18</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="H84" s="10"/>
-      <c r="I84" s="10"/>
-      <c r="J84" s="10"/>
-      <c r="K84" s="10"/>
-      <c r="L84" s="10"/>
-      <c r="M84" s="10"/>
-      <c r="N84" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
     </row>
     <row r="85" spans="1:14" ht="108" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C85" s="11">
+      <c r="C85" s="10">
         <v>18</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>128</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="H85" s="10"/>
-      <c r="I85" s="10"/>
-      <c r="J85" s="10"/>
-      <c r="K85" s="10"/>
-      <c r="L85" s="10"/>
-      <c r="M85" s="10"/>
-      <c r="N85" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final changes with new id
</commit_message>
<xml_diff>
--- a/FieldConfigrationFile.xlsx
+++ b/FieldConfigrationFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prakhar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P_Singh07\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0EFA961-567C-426E-AAFF-9E1676B504E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FD32C5A-B07C-4D86-A961-FC517DD9948D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{02CFE6FC-DC13-4DF7-B179-54CE07624848}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11385" xr2:uid="{02CFE6FC-DC13-4DF7-B179-54CE07624848}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -949,7 +949,284 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">In the </t>
+      <t xml:space="preserve">In the CAM Excel file, within the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Basic Input sheet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> under the Proposed Loan Breakup section, there is a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field called “Type of Loan.”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This field typically contains values such as Home Loan.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>In the PD (Word document), within the Proposed Loan Breakup table, there is a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field  “Type of Loan.”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This field generally includes values such as Home Loan, Composite Loan (Plot Purchase plus Home Construction), and similar options.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, at the beginning of the document, there is a section titled </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Loan Details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Under this section, you will find a field named </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Scheme,”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which typically contains values such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PLOT AND </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HOME CONSTRUCTION LOAN,  PLOT HOME CONSTRUCTION LOAN among others.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>In the PD report, under the Applicant Details section, there is a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> labeled “</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Profile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,” which generally contains values such as Salaried, among others.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Occupation/Business Details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, the field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Salaried / Self-Employed”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically contains values such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Salaried</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SENP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and other similar categories.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the CAM file, under the </t>
     </r>
     <r>
       <rPr>
@@ -970,274 +1247,180 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> sheet under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Proposed Loan Break-up”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section, extract the value from the field </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Proposed ROI.”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> This value is typically presented in formats like </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10.50%</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12.00% etc.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Proposed Loan Break-up” section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which will be tabular form, refer to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>field name “Proposed ROI,”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> where the value will appear in formats such as 10.50% or 12.00% etc</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the CAM Excel file, within the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Basic Input sheet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> under the Proposed Loan Breakup section, there is a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field called “Type of Loan.”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> This field typically contains values such as Home Loan.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>In the PD (Word document), within the Proposed Loan Breakup table, there is a</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field  “Type of Loan.”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> This field generally includes values such as Home Loan, Composite Loan (Plot Purchase plus Home Construction), and similar options.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, at the beginning of the document, there is a section titled </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Loan Details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Under this section, you will find a field named </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Scheme,”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which typically contains values such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">PLOT AND </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> HOME CONSTRUCTION LOAN,  PLOT HOME CONSTRUCTION LOAN among others.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>In the PD report, under the Applicant Details section, there is a</t>
+      <t xml:space="preserve"> sheet and the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Parties to the Loan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Name”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically contains values such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vikram Singh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Girish Kumar Nanda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mohd. Azhar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and similar entries.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Personal Details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, the</t>
     </r>
     <r>
       <rPr>
@@ -1258,28 +1441,91 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> labeled “</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Profile</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,” which generally contains values such as Salaried, among others.</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Name”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will contain values such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vikram Singh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Girish Kumar Nanda</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mohd. Azhar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and similar applicant names.</t>
     </r>
   </si>
   <si>
@@ -1295,28 +1541,248 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Occupation/Business Details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section, the field </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Salaried / Self-Employed”</t>
+      <t>Personal Details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Date of Birth”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> usually values appears in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DD/MM/YYYY</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> format, with sample values such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>02/01/2024</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>24/03/1991</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and similar dates.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the PD document, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Applicant Details section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>review the details of the second applicant.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> There, you will find a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field name “Relationship”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which typically includes values such as Spouse, Mother, and similar relationships.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current/Communication Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“City”</t>
     </r>
     <r>
       <rPr>
@@ -1337,7 +1803,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Salaried</t>
+      <t>Bhopal</t>
     </r>
     <r>
       <rPr>
@@ -1358,127 +1824,75 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SENP</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and other similar categories.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>In the CAM file, under the AffordableCMAssessedIncome sheet, the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field “FOIR for Applied Loan Amount”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically contains values such as 44.55%, 33.24%, and similar percentages.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the PD (Word document), under the Income Details section, which contains tabular data, the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>field “FOIR for Applied Loan Amount”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically includes values such as 55.02%, 33.24%, and similar percentages.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the CAM file, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Basic Input</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sheet and the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Parties to the Loan</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the field</t>
+      <t>Indore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lucknow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and similar city names.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current/Communication Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the field</t>
     </r>
     <r>
       <rPr>
@@ -1499,7 +1913,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>“Name”</t>
+      <t>“Pincode”</t>
     </r>
     <r>
       <rPr>
@@ -1520,7 +1934,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Vikram Singh</t>
+      <t>226024</t>
     </r>
     <r>
       <rPr>
@@ -1541,7 +1955,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Girish Kumar Nanda</t>
+      <t>110024</t>
     </r>
     <r>
       <rPr>
@@ -1562,117 +1976,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mohd. Azhar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and similar entries.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Personal Details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Name”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> will contain values such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vikram Singh</t>
+      <t>201010</t>
     </r>
     <r>
       <rPr>
@@ -1693,556 +1997,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Girish Kumar Nanda</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mohd. Azhar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and similar applicant names.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Personal Details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section, the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Date of Birth”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> usually values appears in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DD/MM/YYYY</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> format, with sample values such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>02/01/2024</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>24/03/1991</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and similar dates.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the PD document, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Applicant Details section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>review the details of the second applicant.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> There, you will find a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>field name “Relationship”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> which typically includes values such as Spouse, Mother, and similar relationships.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Current/Communication Address section</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> fields Address 1, Address 2, and Address 3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically contain address details such as Ashoka Society, Arera Colony, H. No. E7/112, Bhopal, or similar address information.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Current/Communication Address</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“City”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically contains values such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Bhopal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Indore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lucknow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and similar city names.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Current/Communication Address</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Pincode”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically contains values such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>226024</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>110024</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>201010</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>400503</t>
     </r>
     <r>
@@ -2254,137 +2008,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>, and similar numeric codes.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Current/Communication Address</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> section, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the field</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Mobile No.”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically contains values such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8377998214</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>9876543210</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7823445432</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and other similar mobile numbers.</t>
     </r>
   </si>
   <si>
@@ -7605,158 +7228,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> section, the fields </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Office Address 1,” “Office Address 2,”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>“Office Address 3”</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> typically contain address details such as </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Kishanganj Thana, Mhow</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Indore</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Madhya Pradesh</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>452001</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, and similar office address information.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">In the Application Form, under the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Occupation/Business Details</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> section, the </t>
     </r>
     <r>
@@ -11574,7 +11045,522 @@
     </r>
   </si>
   <si>
-    <t>Mismatch Criticality</t>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current/Communication Address section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fields Address 1, Address 2, and Address 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically contain address details such as Ashoka Society, Arera Colony, H. No. E7/112, Bhopal, or similar address information.
+While extracting the address, do not include commas (,) in the final output. If commas appear in the source value, remove them.
+Example:
+If Source: H. No. E7/112, Arera Colony, Bhopal
+then Output: H. No. E7/112 Arera Colony Bhopal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Occupation/Business Details</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, the fields </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Office Address 1,” “Office Address 2,”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Office Address 3”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically contain address details such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kishanganj Thana, Mhow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Indore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Madhya Pradesh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>452001</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and similar office address information.
+While extracting the address, do not include commas (,) in the final output. If commas appear in the source value, remove them.
+Example:
+if Source: H. No. E7/112, Arera Colony, Bhopal
+then Output: H. No. E7/112 Arera Colony Bhopal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the Application Form, under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Current/Communication Address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>the field</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Mobile No.”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically contains values such as </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+91 8377998214, +919876543210, 7823445432</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and other similar mobile numbers.
+While extracting the mobile number, do not include the country code (+91). If the country code is present, remove it and return only the 10-digit mobile number.
+Example:
+Source: +91 8377998214
+Output: 8377998214</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Basic Input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Proposed Loan Break-up”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> section, extract the value from the field </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Proposed ROI.”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> This value is typically presented in formats like </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10.50%</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12.00% etc.
+While extracting the value, do not include the percentage (%) sign. Remove the % symbol and return only the numeric value.
+Example:
+Source: 10.50%
+Output: 10.50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>“Proposed Loan Break-up” section</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which will be tabular form, refer to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field name “Proposed ROI,”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> where the value will appear in formats such as 10.50% or 12.00% etc
+While extracting the value, do not include the percentage (%) sign. Remove the % symbol and return only the numeric value.
+Example:
+Source: 10.50%
+Output: 10.50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>In the CAM file, under the AffordableCMAssessedIncome sheet, the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field “FOIR for Applied Loan Amount”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically contains values such as 44.55%, 33.24%, and similar percentages.
+While extracting the value, do not include the percentage (%) sign. Remove the % symbol and return only the numeric value.
+Example:
+Source: 10.50%
+Output: 10.50</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the PD (Word document), under the Income Details section, which contains tabular data, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>field “FOIR for Applied Loan Amount”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> typically includes values such as 55.02%, 33.24%, and similar percentages.
+While extracting the value, do not include the percentage (%) sign. Remove the % symbol and return only the numeric value.
+Example:
+Source: 10.50%
+Output: 10.50</t>
+    </r>
+  </si>
+  <si>
+    <t>Criticality</t>
   </si>
 </sst>
 </file>
@@ -12053,8 +12039,8 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12133,10 +12119,10 @@
         <v>126</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
@@ -12167,7 +12153,7 @@
         <v>126</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="9"/>
@@ -12195,10 +12181,10 @@
         <v>126</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -12229,10 +12215,10 @@
         <v>126</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -12263,7 +12249,7 @@
         <v>126</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="9"/>
@@ -12291,25 +12277,25 @@
         <v>126</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="N7" s="9"/>
     </row>
@@ -12327,10 +12313,10 @@
         <v>126</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>136</v>
@@ -12349,7 +12335,7 @@
       </c>
       <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="168" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -12363,17 +12349,17 @@
         <v>126</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>140</v>
+        <v>249</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="s">
-        <v>141</v>
+        <v>250</v>
       </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
@@ -12395,20 +12381,20 @@
         <v>126</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
@@ -12429,29 +12415,29 @@
         <v>126</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>109</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>110</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
     </row>
-    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="156" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
@@ -12465,19 +12451,19 @@
         <v>126</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>147</v>
+        <v>251</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>148</v>
+        <v>252</v>
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -12499,18 +12485,18 @@
         <v>126</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
@@ -12531,18 +12517,18 @@
         <v>126</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -12563,14 +12549,14 @@
         <v>126</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
@@ -12591,16 +12577,16 @@
         <v>126</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -12609,7 +12595,7 @@
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="1:14" ht="84" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="204" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
@@ -12623,14 +12609,14 @@
         <v>127</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="s">
-        <v>153</v>
+        <v>246</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -12651,14 +12637,14 @@
         <v>126</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
@@ -12679,21 +12665,21 @@
         <v>126</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
     </row>
-    <row r="20" spans="1:14" ht="72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
@@ -12707,14 +12693,14 @@
         <v>126</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="9" t="s">
-        <v>156</v>
+        <v>248</v>
       </c>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -12735,10 +12721,10 @@
         <v>126</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9" t="s">
@@ -12767,20 +12753,20 @@
         <v>126</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -12801,14 +12787,14 @@
         <v>126</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
@@ -12829,12 +12815,12 @@
         <v>127</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -12857,20 +12843,20 @@
         <v>127</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
@@ -12891,11 +12877,11 @@
         <v>126</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
@@ -12919,11 +12905,11 @@
         <v>126</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="9" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
@@ -12947,20 +12933,20 @@
         <v>126</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -12981,20 +12967,20 @@
         <v>126</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
@@ -13015,14 +13001,14 @@
         <v>127</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -13045,14 +13031,14 @@
         <v>126</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
@@ -13075,17 +13061,17 @@
         <v>127</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="11" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -13107,17 +13093,17 @@
         <v>127</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -13139,14 +13125,14 @@
         <v>126</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>123</v>
@@ -13171,13 +13157,13 @@
         <v>127</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="9"/>
@@ -13201,10 +13187,10 @@
         <v>127</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>124</v>
@@ -13231,13 +13217,13 @@
         <v>127</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
@@ -13261,13 +13247,13 @@
         <v>127</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
@@ -13291,13 +13277,13 @@
         <v>127</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
@@ -13321,18 +13307,18 @@
         <v>126</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="9"/>
       <c r="J40" s="9" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
@@ -13353,11 +13339,11 @@
         <v>126</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F41" s="8"/>
       <c r="G41" s="11" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
@@ -13381,11 +13367,11 @@
         <v>127</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F42" s="8"/>
       <c r="G42" s="9" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
@@ -13409,16 +13395,16 @@
         <v>126</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="H43" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -13441,13 +13427,13 @@
         <v>126</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
@@ -13471,11 +13457,11 @@
         <v>126</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="9" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
@@ -13499,7 +13485,7 @@
         <v>126</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F46" s="8"/>
       <c r="G46" s="9"/>
@@ -13507,7 +13493,7 @@
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
@@ -13527,11 +13513,11 @@
         <v>127</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F47" s="8"/>
       <c r="G47" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
@@ -13555,11 +13541,11 @@
         <v>127</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F48" s="8"/>
       <c r="G48" s="9" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
@@ -13583,13 +13569,13 @@
         <v>126</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
@@ -13613,17 +13599,17 @@
         <v>127</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
@@ -13643,7 +13629,7 @@
         <v>126</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="9"/>
@@ -13651,7 +13637,7 @@
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
@@ -13671,10 +13657,10 @@
         <v>126</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G52" s="9"/>
       <c r="H52" s="9" t="s">
@@ -13703,14 +13689,14 @@
         <v>126</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
@@ -13731,20 +13717,20 @@
         <v>126</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
@@ -13765,20 +13751,20 @@
         <v>127</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G55" s="9"/>
       <c r="H55" s="9" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="I55" s="9" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
@@ -13799,15 +13785,15 @@
         <v>126</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F56" s="8"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
@@ -13829,18 +13815,18 @@
         <v>126</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G57" s="9"/>
       <c r="H57" s="9" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I57" s="9"/>
       <c r="J57" s="9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
@@ -13861,20 +13847,20 @@
         <v>126</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G58" s="9"/>
       <c r="H58" s="9" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="I58" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -13895,27 +13881,27 @@
         <v>126</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G59" s="9"/>
       <c r="H59" s="9" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="I59" s="9" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
     </row>
-    <row r="60" spans="1:14" ht="96" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="216" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>67</v>
       </c>
@@ -13929,14 +13915,14 @@
         <v>127</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F60" s="8"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
@@ -13957,14 +13943,14 @@
         <v>127</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F61" s="8"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
@@ -13985,11 +13971,11 @@
         <v>127</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F62" s="8"/>
       <c r="G62" s="9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="9"/>
@@ -14013,14 +13999,14 @@
         <v>127</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G63" s="9"/>
       <c r="H63" s="11" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
@@ -14043,13 +14029,13 @@
         <v>127</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
@@ -14073,13 +14059,13 @@
         <v>126</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="9"/>
@@ -14103,13 +14089,13 @@
         <v>126</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H66" s="9"/>
       <c r="I66" s="9"/>
@@ -14133,13 +14119,13 @@
         <v>126</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
@@ -14163,13 +14149,13 @@
         <v>126</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H68" s="9"/>
       <c r="I68" s="9"/>
@@ -14193,13 +14179,13 @@
         <v>126</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="9"/>
@@ -14223,13 +14209,13 @@
         <v>127</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
@@ -14253,13 +14239,13 @@
         <v>127</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H71" s="9"/>
       <c r="I71" s="9"/>
@@ -14283,13 +14269,13 @@
         <v>127</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
@@ -14313,13 +14299,13 @@
         <v>127</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
@@ -14343,13 +14329,13 @@
         <v>126</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
@@ -14373,13 +14359,13 @@
         <v>126</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
@@ -14403,13 +14389,13 @@
         <v>127</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
@@ -14433,13 +14419,13 @@
         <v>127</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
@@ -14463,11 +14449,11 @@
         <v>127</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F78" s="8"/>
       <c r="G78" s="9" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
@@ -14491,11 +14477,11 @@
         <v>127</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F79" s="8"/>
       <c r="G79" s="9" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="H79" s="9"/>
       <c r="I79" s="9"/>
@@ -14519,11 +14505,11 @@
         <v>127</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F80" s="8"/>
       <c r="G80" s="9" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
@@ -14547,11 +14533,11 @@
         <v>127</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F81" s="8"/>
       <c r="G81" s="9" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
@@ -14575,17 +14561,17 @@
         <v>127</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="H82" s="9"/>
       <c r="I82" s="9" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
@@ -14607,13 +14593,13 @@
         <v>127</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F83" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
@@ -14637,13 +14623,13 @@
         <v>127</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F84" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
@@ -14667,13 +14653,13 @@
         <v>127</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="H85" s="9"/>
       <c r="I85" s="9"/>

</xml_diff>